<commit_message>
Added NovelLife Clock and option for hardcoded WIFI
Added Pinout for NovelLife to global defines
Option to skip WPS and use hardcoded WIFI creds
Added SECRETS.h to save WIFI creds and API keys with example file
</commit_message>
<xml_diff>
--- a/Hardware pinout.xlsx
+++ b/Hardware pinout.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OGRIN\Dropbox\EleksTubeIPS\EleksTubeHAX_AO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\devel\EleksTubeHAX-main\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7899FC6B-57DF-4437-A31F-C745219448D4}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E3B617E-028B-453C-A436-91508E4C4E95}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18576" yWindow="84" windowWidth="40068" windowHeight="15576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="All the pins" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="385" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="418" uniqueCount="276">
   <si>
     <t>No.</t>
   </si>
@@ -839,13 +839,22 @@
   </si>
   <si>
     <t>DSP 11 TFT - CLOCK</t>
+  </si>
+  <si>
+    <t>WROVER NC</t>
+  </si>
+  <si>
+    <t>Novellife SE</t>
+  </si>
+  <si>
+    <t>Stupid gesture sensor -- not interested in making it work</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -905,6 +914,12 @@
       <family val="2"/>
       <charset val="238"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -959,64 +974,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+  <cellXfs count="30">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1028,8 +1020,11 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1250,1975 +1245,2046 @@
   </sheetPr>
   <dimension ref="A1:U56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" customWidth="1"/>
-    <col min="2" max="2" width="11.5703125" customWidth="1"/>
-    <col min="3" max="3" width="5.7109375" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" customWidth="1"/>
+    <col min="1" max="1" width="4.44140625" customWidth="1"/>
+    <col min="2" max="2" width="11.5546875" customWidth="1"/>
+    <col min="3" max="3" width="5.6640625" customWidth="1"/>
+    <col min="4" max="4" width="7.5546875" customWidth="1"/>
     <col min="5" max="5" width="12" customWidth="1"/>
-    <col min="6" max="6" width="16.7109375" customWidth="1"/>
-    <col min="7" max="7" width="11.42578125" style="10" customWidth="1"/>
-    <col min="8" max="8" width="8.28515625" customWidth="1"/>
-    <col min="9" max="9" width="6.85546875" customWidth="1"/>
-    <col min="10" max="10" width="5.5703125" customWidth="1"/>
+    <col min="6" max="6" width="16.6640625" customWidth="1"/>
+    <col min="7" max="7" width="11.44140625" customWidth="1"/>
+    <col min="8" max="8" width="8.33203125" customWidth="1"/>
+    <col min="9" max="9" width="6.88671875" customWidth="1"/>
+    <col min="10" max="10" width="5.5546875" customWidth="1"/>
     <col min="11" max="11" width="6" customWidth="1"/>
-    <col min="12" max="12" width="12.85546875" customWidth="1"/>
+    <col min="12" max="12" width="12.88671875" customWidth="1"/>
     <col min="13" max="13" width="7" customWidth="1"/>
-    <col min="14" max="14" width="13.140625" customWidth="1"/>
-    <col min="15" max="15" width="6.7109375" customWidth="1"/>
-    <col min="16" max="16" width="11.28515625" customWidth="1"/>
-    <col min="17" max="17" width="15.28515625" customWidth="1"/>
-    <col min="18" max="18" width="30.28515625" customWidth="1"/>
+    <col min="14" max="14" width="13.109375" customWidth="1"/>
+    <col min="15" max="15" width="6.6640625" customWidth="1"/>
+    <col min="16" max="16" width="11.33203125" customWidth="1"/>
+    <col min="17" max="17" width="15.33203125" customWidth="1"/>
+    <col min="18" max="18" width="30.33203125" customWidth="1"/>
     <col min="19" max="20" width="27" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="13" customFormat="1" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="37" t="s">
+    <row r="1" spans="1:21" s="6" customFormat="1" ht="46.8" x14ac:dyDescent="0.3">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="23" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37" t="s">
+      <c r="C1" s="23" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="37" t="s">
+      <c r="D1" s="23" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="37" t="s">
+      <c r="E1" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="37" t="s">
+      <c r="F1" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="38" t="s">
+      <c r="G1" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="37" t="s">
+      <c r="H1" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="37" t="s">
+      <c r="I1" s="23" t="s">
         <v>8</v>
       </c>
-      <c r="J1" s="37" t="s">
+      <c r="J1" s="23" t="s">
         <v>9</v>
       </c>
-      <c r="K1" s="37" t="s">
+      <c r="K1" s="23" t="s">
         <v>10</v>
       </c>
-      <c r="L1" s="37" t="s">
+      <c r="L1" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="37" t="s">
+      <c r="M1" s="23" t="s">
         <v>11</v>
       </c>
-      <c r="N1" s="37" t="s">
+      <c r="N1" s="23" t="s">
         <v>12</v>
       </c>
-      <c r="O1" s="37" t="s">
+      <c r="O1" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="P1" s="37" t="s">
+      <c r="P1" s="23" t="s">
         <v>14</v>
       </c>
-      <c r="Q1" s="37" t="s">
+      <c r="Q1" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="R1" s="39" t="s">
+      <c r="R1" s="24" t="s">
         <v>219</v>
       </c>
-      <c r="S1" s="37" t="s">
+      <c r="S1" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="T1" s="37" t="s">
+      <c r="T1" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="U1" s="12"/>
-    </row>
-    <row r="2" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="5">
+      <c r="U1" s="23" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="2" spans="1:21" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="3">
         <v>1</v>
       </c>
-      <c r="B2" s="5" t="s">
+      <c r="B2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="C2" s="5" t="s">
+      <c r="C2" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="5"/>
-      <c r="F2" s="5"/>
-      <c r="G2" s="8"/>
-      <c r="H2" s="5"/>
-      <c r="I2" s="5"/>
-      <c r="J2" s="5"/>
-      <c r="K2" s="5"/>
-      <c r="L2" s="5"/>
-      <c r="M2" s="5"/>
-      <c r="N2" s="5"/>
-      <c r="O2" s="5"/>
-      <c r="P2" s="5"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5" t="s">
+      <c r="D2" s="3"/>
+      <c r="E2" s="3"/>
+      <c r="F2" s="3"/>
+      <c r="G2" s="3"/>
+      <c r="H2" s="3"/>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3"/>
+      <c r="K2" s="3"/>
+      <c r="L2" s="3"/>
+      <c r="M2" s="3"/>
+      <c r="N2" s="3"/>
+      <c r="O2" s="3"/>
+      <c r="P2" s="3"/>
+      <c r="Q2" s="3"/>
+      <c r="R2" s="3"/>
+      <c r="S2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="T2" s="5" t="s">
+      <c r="T2" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="U2" s="6"/>
-    </row>
-    <row r="3" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="U2" s="3" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="3" spans="1:21" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="3">
         <v>2</v>
       </c>
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="C3" s="5" t="s">
+      <c r="C3" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="8"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
-      <c r="K3" s="5"/>
-      <c r="L3" s="5"/>
-      <c r="M3" s="5"/>
-      <c r="N3" s="5"/>
-      <c r="O3" s="5"/>
-      <c r="P3" s="5"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5" t="s">
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="3"/>
+      <c r="I3" s="3"/>
+      <c r="J3" s="3"/>
+      <c r="K3" s="3"/>
+      <c r="L3" s="3"/>
+      <c r="M3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="O3" s="3"/>
+      <c r="P3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="R3" s="3"/>
+      <c r="S3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="T3" s="5" t="s">
+      <c r="T3" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="U3" s="6"/>
-    </row>
-    <row r="4" spans="1:21" s="7" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="19">
+      <c r="U3" s="3" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="4" spans="1:21" s="5" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="12">
         <v>3</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="12" t="s">
         <v>197</v>
       </c>
-      <c r="D4" s="19"/>
-      <c r="E4" s="19"/>
-      <c r="F4" s="19"/>
-      <c r="G4" s="19"/>
-      <c r="H4" s="19"/>
-      <c r="I4" s="19"/>
-      <c r="J4" s="19"/>
-      <c r="K4" s="19"/>
-      <c r="L4" s="19"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="19"/>
-      <c r="O4" s="19"/>
-      <c r="P4" s="19"/>
-      <c r="Q4" s="19"/>
-      <c r="R4" s="19"/>
-      <c r="S4" s="19" t="s">
+      <c r="D4" s="12"/>
+      <c r="E4" s="12"/>
+      <c r="F4" s="12"/>
+      <c r="G4" s="12"/>
+      <c r="H4" s="12"/>
+      <c r="I4" s="12"/>
+      <c r="J4" s="12"/>
+      <c r="K4" s="12"/>
+      <c r="L4" s="12"/>
+      <c r="M4" s="12"/>
+      <c r="N4" s="12"/>
+      <c r="O4" s="12"/>
+      <c r="P4" s="12"/>
+      <c r="Q4" s="12"/>
+      <c r="R4" s="12"/>
+      <c r="S4" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="12" t="s">
         <v>214</v>
       </c>
-      <c r="U4" s="6"/>
-    </row>
-    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="4">
+      <c r="U4" s="12" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="5" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="2">
         <v>4</v>
       </c>
-      <c r="B5" s="3" t="s">
+      <c r="B5" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C5" s="3" t="s">
+      <c r="C5" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D5" s="3" t="s">
+      <c r="D5" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="E5" s="3" t="s">
+      <c r="E5" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F5" s="3" t="s">
+      <c r="F5" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="G5" s="9" t="s">
+      <c r="G5" s="1" t="s">
         <v>209</v>
       </c>
-      <c r="H5" s="3"/>
-      <c r="I5" s="3"/>
-      <c r="J5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="L5" s="3"/>
-      <c r="M5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="O5" s="3"/>
-      <c r="P5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="R5" s="3" t="s">
+      <c r="H5" s="1"/>
+      <c r="I5" s="1"/>
+      <c r="J5" s="1"/>
+      <c r="K5" s="1"/>
+      <c r="L5" s="1"/>
+      <c r="M5" s="1"/>
+      <c r="N5" s="1"/>
+      <c r="O5" s="1"/>
+      <c r="P5" s="1"/>
+      <c r="Q5" s="1"/>
+      <c r="R5" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="S5" s="6" t="s">
+      <c r="S5" s="4" t="s">
         <v>224</v>
       </c>
-      <c r="T5" s="6" t="s">
+      <c r="T5" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="U5" s="1"/>
-    </row>
-    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="4">
+      <c r="U5" s="29" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="6" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="2">
         <v>5</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="B6" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="C6" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="1" t="s">
         <v>211</v>
       </c>
-      <c r="E6" s="3" t="s">
+      <c r="E6" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="3" t="s">
+      <c r="F6" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="G6" s="9" t="s">
+      <c r="G6" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="L6" s="3"/>
-      <c r="M6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="O6" s="3"/>
-      <c r="P6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="R6" s="3" t="s">
+      <c r="H6" s="1"/>
+      <c r="I6" s="1"/>
+      <c r="J6" s="1"/>
+      <c r="K6" s="1"/>
+      <c r="L6" s="1"/>
+      <c r="M6" s="1"/>
+      <c r="N6" s="1"/>
+      <c r="O6" s="1"/>
+      <c r="P6" s="1"/>
+      <c r="Q6" s="1"/>
+      <c r="R6" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="S6" s="6" t="s">
+      <c r="S6" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T6" s="6" t="s">
+      <c r="T6" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="U6" s="2"/>
-    </row>
-    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="4">
+      <c r="U6" s="29"/>
+    </row>
+    <row r="7" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="2">
         <v>6</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="C7" s="3" t="s">
+      <c r="C7" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D7" s="3" t="s">
+      <c r="D7" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="E7" s="3" t="s">
+      <c r="E7" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="F7" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="G7" s="9" t="s">
+      <c r="G7" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="H7" s="3"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="L7" s="3"/>
-      <c r="M7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="3"/>
-      <c r="P7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="R7" s="3" t="s">
+      <c r="H7" s="1"/>
+      <c r="I7" s="1"/>
+      <c r="J7" s="1"/>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
+      <c r="M7" s="1"/>
+      <c r="N7" s="1"/>
+      <c r="O7" s="1"/>
+      <c r="P7" s="1"/>
+      <c r="Q7" s="1"/>
+      <c r="R7" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="S7" s="6" t="s">
+      <c r="S7" s="4" t="s">
         <v>227</v>
       </c>
-      <c r="T7" s="6" t="s">
+      <c r="T7" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="U7" s="2"/>
-    </row>
-    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="4">
+      <c r="U7" s="29"/>
+    </row>
+    <row r="8" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="2">
         <v>7</v>
       </c>
-      <c r="B8" s="3" t="s">
+      <c r="B8" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="C8" s="3" t="s">
+      <c r="C8" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="D8" s="3" t="s">
+      <c r="D8" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="E8" s="3" t="s">
+      <c r="E8" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="3" t="s">
+      <c r="F8" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="G8" s="9" t="s">
+      <c r="G8" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="L8" s="3"/>
-      <c r="M8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="3"/>
-      <c r="P8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="R8" s="3" t="s">
+      <c r="H8" s="1"/>
+      <c r="I8" s="1"/>
+      <c r="J8" s="1"/>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
+      <c r="M8" s="1"/>
+      <c r="N8" s="1"/>
+      <c r="O8" s="1"/>
+      <c r="P8" s="1"/>
+      <c r="Q8" s="1"/>
+      <c r="R8" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="S8" s="6" t="s">
+      <c r="S8" s="4" t="s">
         <v>228</v>
       </c>
-      <c r="T8" s="6" t="s">
+      <c r="T8" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="U8" s="2"/>
-    </row>
-    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="4">
+      <c r="U8" s="29"/>
+    </row>
+    <row r="9" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="2">
         <v>8</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="C9" s="3" t="s">
+      <c r="C9" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="D9" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="E9" s="3"/>
-      <c r="F9" s="3" t="s">
+      <c r="E9" s="1"/>
+      <c r="F9" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="G9" s="9" t="s">
+      <c r="G9" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="H9" s="3" t="s">
+      <c r="H9" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="I9" s="3"/>
-      <c r="J9" s="3"/>
-      <c r="K9" s="3"/>
-      <c r="L9" s="3"/>
-      <c r="M9" s="3"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="3"/>
-      <c r="P9" s="3"/>
-      <c r="Q9" s="3"/>
-      <c r="R9" s="3" t="s">
+      <c r="I9" s="1"/>
+      <c r="J9" s="1"/>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
+      <c r="M9" s="1"/>
+      <c r="N9" s="1"/>
+      <c r="O9" s="1"/>
+      <c r="P9" s="1"/>
+      <c r="Q9" s="1"/>
+      <c r="R9" s="1" t="s">
         <v>189</v>
       </c>
-      <c r="S9" s="6" t="s">
+      <c r="S9" s="4" t="s">
         <v>226</v>
       </c>
-      <c r="T9" s="6" t="s">
+      <c r="T9" s="4" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="4">
+    <row r="10" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="2">
         <v>9</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C10" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="D10" s="1" t="s">
         <v>191</v>
       </c>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3" t="s">
+      <c r="E10" s="1"/>
+      <c r="F10" s="1" t="s">
         <v>192</v>
       </c>
-      <c r="G10" s="9" t="s">
+      <c r="G10" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="H10" s="3" t="s">
+      <c r="H10" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
-      <c r="K10" s="3"/>
-      <c r="L10" s="3"/>
-      <c r="M10" s="3"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="3"/>
-      <c r="P10" s="3"/>
-      <c r="Q10" s="3"/>
-      <c r="R10" s="3" t="s">
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
+      <c r="M10" s="1"/>
+      <c r="N10" s="1"/>
+      <c r="O10" s="1"/>
+      <c r="P10" s="1"/>
+      <c r="Q10" s="1"/>
+      <c r="R10" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="S10" s="6" t="s">
+      <c r="S10" s="4" t="s">
         <v>225</v>
       </c>
-      <c r="T10" s="6" t="s">
+      <c r="T10" s="4" t="s">
         <v>239</v>
       </c>
-      <c r="U10" s="2"/>
-    </row>
-    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="4">
+      <c r="U10" s="1"/>
+    </row>
+    <row r="11" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="2">
         <v>10</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="C11" s="3" t="s">
+      <c r="C11" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="3" t="s">
+      <c r="D11" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3" t="s">
+      <c r="E11" s="1"/>
+      <c r="F11" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="G11" s="9" t="s">
+      <c r="G11" s="1" t="s">
         <v>169</v>
       </c>
-      <c r="H11" s="3"/>
-      <c r="I11" s="3" t="s">
+      <c r="H11" s="1"/>
+      <c r="I11" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="J11" s="3"/>
-      <c r="K11" s="3"/>
-      <c r="L11" s="3"/>
-      <c r="M11" s="3"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="3"/>
-      <c r="P11" s="3"/>
-      <c r="Q11" s="3" t="s">
+      <c r="J11" s="1"/>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
+      <c r="M11" s="1"/>
+      <c r="N11" s="1"/>
+      <c r="O11" s="1"/>
+      <c r="P11" s="1"/>
+      <c r="Q11" s="1" t="s">
         <v>171</v>
       </c>
-      <c r="R11" s="3"/>
-      <c r="S11" s="6" t="s">
+      <c r="R11" s="1"/>
+      <c r="S11" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="T11" s="6" t="s">
+      <c r="T11" s="4" t="s">
         <v>240</v>
       </c>
-      <c r="U11" s="2"/>
-    </row>
-    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="4">
+      <c r="U11" s="4" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="12" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="2">
         <v>11</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="C12" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="D12" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3" t="s">
+      <c r="E12" s="1"/>
+      <c r="F12" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="G12" s="9" t="s">
+      <c r="G12" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3" t="s">
+      <c r="H12" s="1"/>
+      <c r="I12" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="J12" s="3"/>
-      <c r="K12" s="3"/>
-      <c r="L12" s="3"/>
-      <c r="M12" s="3"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="3"/>
-      <c r="P12" s="3"/>
-      <c r="Q12" s="3" t="s">
+      <c r="J12" s="1"/>
+      <c r="K12" s="1"/>
+      <c r="L12" s="1"/>
+      <c r="M12" s="1"/>
+      <c r="N12" s="1"/>
+      <c r="O12" s="1"/>
+      <c r="P12" s="1"/>
+      <c r="Q12" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="R12" s="3"/>
-      <c r="S12" s="6" t="s">
+      <c r="R12" s="1"/>
+      <c r="S12" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="T12" s="6" t="s">
+      <c r="T12" s="4" t="s">
         <v>241</v>
       </c>
-      <c r="U12" s="2"/>
-    </row>
-    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="4">
+      <c r="U12" s="4" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="13" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="2">
         <v>12</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C13" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D13" s="3" t="s">
+      <c r="D13" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="E13" s="3"/>
-      <c r="F13" s="3" t="s">
+      <c r="E13" s="1"/>
+      <c r="F13" s="1" t="s">
         <v>180</v>
       </c>
-      <c r="G13" s="9" t="s">
+      <c r="G13" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="H13" s="3" t="s">
+      <c r="H13" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I13" s="3"/>
-      <c r="J13" s="3"/>
-      <c r="K13" s="3"/>
-      <c r="L13" s="3"/>
-      <c r="M13" s="3"/>
-      <c r="N13" s="3"/>
-      <c r="O13" s="3"/>
-      <c r="P13" s="3"/>
-      <c r="Q13" s="3" t="s">
+      <c r="I13" s="1"/>
+      <c r="J13" s="1"/>
+      <c r="K13" s="1"/>
+      <c r="L13" s="1"/>
+      <c r="M13" s="1"/>
+      <c r="N13" s="1"/>
+      <c r="O13" s="1"/>
+      <c r="P13" s="1"/>
+      <c r="Q13" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="R13" s="3"/>
-      <c r="S13" s="6" t="s">
+      <c r="R13" s="1"/>
+      <c r="S13" s="4" t="s">
         <v>235</v>
       </c>
-      <c r="T13" s="6" t="s">
+      <c r="T13" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="U13" s="2"/>
-    </row>
-    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="4">
+      <c r="U13" s="4"/>
+    </row>
+    <row r="14" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="2">
         <v>13</v>
       </c>
-      <c r="B14" s="3" t="s">
+      <c r="B14" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="C14" s="3" t="s">
+      <c r="C14" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="3" t="s">
+      <c r="D14" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3" t="s">
+      <c r="E14" s="1"/>
+      <c r="F14" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="G14" s="9" t="s">
+      <c r="G14" s="1" t="s">
         <v>110</v>
       </c>
-      <c r="H14" s="3" t="s">
+      <c r="H14" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-      <c r="K14" s="3"/>
-      <c r="L14" s="3" t="s">
+      <c r="I14" s="1"/>
+      <c r="J14" s="1"/>
+      <c r="K14" s="1"/>
+      <c r="L14" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="M14" s="3"/>
-      <c r="N14" s="3" t="s">
+      <c r="M14" s="1"/>
+      <c r="N14" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="O14" s="3" t="s">
+      <c r="O14" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="P14" s="3"/>
-      <c r="Q14" s="3" t="s">
+      <c r="P14" s="1"/>
+      <c r="Q14" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="R14" s="3"/>
-      <c r="S14" s="3" t="s">
+      <c r="R14" s="1"/>
+      <c r="S14" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="T14" s="6" t="s">
+      <c r="T14" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="U14" s="2"/>
-    </row>
-    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="23">
+      <c r="U14" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="15" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="16">
         <v>14</v>
       </c>
-      <c r="B15" s="24" t="s">
+      <c r="B15" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="24" t="s">
+      <c r="C15" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D15" s="24" t="s">
+      <c r="D15" s="17" t="s">
         <v>90</v>
       </c>
-      <c r="E15" s="24" t="s">
+      <c r="E15" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F15" s="24" t="s">
+      <c r="F15" s="17" t="s">
         <v>91</v>
       </c>
-      <c r="G15" s="24" t="s">
+      <c r="G15" s="17" t="s">
         <v>92</v>
       </c>
-      <c r="H15" s="24" t="s">
+      <c r="H15" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="I15" s="24"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="24"/>
-      <c r="L15" s="24" t="s">
+      <c r="I15" s="17"/>
+      <c r="J15" s="17"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="17" t="s">
         <v>94</v>
       </c>
-      <c r="M15" s="24"/>
-      <c r="N15" s="24" t="s">
+      <c r="M15" s="17"/>
+      <c r="N15" s="17" t="s">
         <v>95</v>
       </c>
-      <c r="O15" s="24" t="s">
+      <c r="O15" s="17" t="s">
         <v>96</v>
       </c>
-      <c r="P15" s="24"/>
-      <c r="Q15" s="24" t="s">
+      <c r="P15" s="17"/>
+      <c r="Q15" s="17" t="s">
         <v>97</v>
       </c>
-      <c r="R15" s="25" t="s">
+      <c r="R15" s="18" t="s">
         <v>220</v>
       </c>
-      <c r="S15" s="27" t="s">
+      <c r="S15" s="19" t="s">
         <v>234</v>
       </c>
-      <c r="T15" s="27" t="s">
+      <c r="T15" s="19" t="s">
         <v>263</v>
       </c>
-      <c r="U15" s="2"/>
-    </row>
-    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="32">
+      <c r="U15" s="19" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="16" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="2">
         <v>15</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="C16" s="34" t="s">
+      <c r="C16" s="3" t="s">
         <v>218</v>
       </c>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="36"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="35"/>
-      <c r="J16" s="35"/>
-      <c r="K16" s="35"/>
-      <c r="L16" s="35"/>
-      <c r="M16" s="35"/>
-      <c r="N16" s="35"/>
-      <c r="O16" s="35"/>
-      <c r="P16" s="35"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="35"/>
-      <c r="S16" s="33" t="s">
+      <c r="D16" s="1"/>
+      <c r="E16" s="1"/>
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+      <c r="I16" s="1"/>
+      <c r="J16" s="1"/>
+      <c r="K16" s="1"/>
+      <c r="L16" s="1"/>
+      <c r="M16" s="1"/>
+      <c r="N16" s="1"/>
+      <c r="O16" s="1"/>
+      <c r="P16" s="1"/>
+      <c r="Q16" s="1"/>
+      <c r="R16" s="1"/>
+      <c r="S16" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="T16" s="33" t="s">
+      <c r="T16" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="U16" s="3"/>
-    </row>
-    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="32">
+      <c r="U16" s="4" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="17" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="2">
         <v>16</v>
       </c>
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C17" s="35" t="s">
+      <c r="C17" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D17" s="35" t="s">
+      <c r="D17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E17" s="35"/>
-      <c r="F17" s="35" t="s">
+      <c r="E17" s="1"/>
+      <c r="F17" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="G17" s="36" t="s">
+      <c r="G17" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="H17" s="35" t="s">
+      <c r="H17" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I17" s="35"/>
-      <c r="J17" s="35"/>
-      <c r="K17" s="35"/>
-      <c r="L17" s="35" t="s">
+      <c r="I17" s="1"/>
+      <c r="J17" s="1"/>
+      <c r="K17" s="1"/>
+      <c r="L17" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="M17" s="35"/>
-      <c r="N17" s="35" t="s">
+      <c r="M17" s="1"/>
+      <c r="N17" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="O17" s="35" t="s">
+      <c r="O17" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="P17" s="35"/>
-      <c r="Q17" s="35" t="s">
+      <c r="P17" s="1"/>
+      <c r="Q17" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="R17" s="35"/>
-      <c r="S17" s="6" t="s">
+      <c r="R17" s="1"/>
+      <c r="S17" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T17" s="6" t="s">
+      <c r="T17" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U17" s="2"/>
-    </row>
-    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="14">
+      <c r="U17" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="18" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="7">
         <v>17</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="C18" s="15" t="s">
+      <c r="C18" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D18" s="15" t="s">
+      <c r="D18" s="8" t="s">
         <v>73</v>
       </c>
-      <c r="E18" s="15" t="s">
+      <c r="E18" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F18" s="15" t="s">
+      <c r="F18" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G18" s="16"/>
-      <c r="H18" s="16"/>
-      <c r="I18" s="15"/>
-      <c r="J18" s="15"/>
-      <c r="K18" s="15"/>
-      <c r="L18" s="15" t="s">
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="8"/>
+      <c r="J18" s="8"/>
+      <c r="K18" s="8"/>
+      <c r="L18" s="8" t="s">
         <v>77</v>
       </c>
-      <c r="M18" s="15" t="s">
+      <c r="M18" s="8" t="s">
         <v>74</v>
       </c>
-      <c r="N18" s="15" t="s">
+      <c r="N18" s="8" t="s">
         <v>75</v>
       </c>
-      <c r="O18" s="15"/>
-      <c r="P18" s="15" t="s">
+      <c r="O18" s="8"/>
+      <c r="P18" s="8" t="s">
         <v>76</v>
       </c>
-      <c r="Q18" s="15"/>
-      <c r="R18" s="3"/>
-      <c r="S18" s="6" t="s">
+      <c r="Q18" s="8"/>
+      <c r="R18" s="1"/>
+      <c r="S18" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T18" s="6" t="s">
+      <c r="T18" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U18" s="2"/>
-    </row>
-    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="14">
+      <c r="U18" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="19" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="7">
         <v>18</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="8" t="s">
         <v>78</v>
       </c>
-      <c r="C19" s="15" t="s">
+      <c r="C19" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D19" s="15" t="s">
+      <c r="D19" s="8" t="s">
         <v>79</v>
       </c>
-      <c r="E19" s="15" t="s">
+      <c r="E19" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F19" s="15" t="s">
+      <c r="F19" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G19" s="16"/>
-      <c r="H19" s="16"/>
-      <c r="I19" s="15"/>
-      <c r="J19" s="15"/>
-      <c r="K19" s="15"/>
-      <c r="L19" s="15" t="s">
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="8"/>
+      <c r="J19" s="8"/>
+      <c r="K19" s="8"/>
+      <c r="L19" s="8" t="s">
         <v>83</v>
       </c>
-      <c r="M19" s="15" t="s">
+      <c r="M19" s="8" t="s">
         <v>80</v>
       </c>
-      <c r="N19" s="15" t="s">
+      <c r="N19" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="O19" s="15"/>
-      <c r="P19" s="15" t="s">
+      <c r="O19" s="8"/>
+      <c r="P19" s="8" t="s">
         <v>82</v>
       </c>
-      <c r="Q19" s="15"/>
-      <c r="R19" s="3"/>
-      <c r="S19" s="6" t="s">
+      <c r="Q19" s="8"/>
+      <c r="R19" s="1"/>
+      <c r="S19" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T19" s="6" t="s">
+      <c r="T19" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U19" s="2"/>
-    </row>
-    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="14">
+      <c r="U19" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="20" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
         <v>19</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="8" t="s">
         <v>84</v>
       </c>
-      <c r="C20" s="15" t="s">
+      <c r="C20" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D20" s="15" t="s">
+      <c r="D20" s="8" t="s">
         <v>85</v>
       </c>
-      <c r="E20" s="15" t="s">
+      <c r="E20" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F20" s="15" t="s">
+      <c r="F20" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G20" s="16"/>
-      <c r="H20" s="16"/>
-      <c r="I20" s="15"/>
-      <c r="J20" s="15"/>
-      <c r="K20" s="15"/>
-      <c r="L20" s="15" t="s">
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="8"/>
+      <c r="J20" s="8"/>
+      <c r="K20" s="8"/>
+      <c r="L20" s="8" t="s">
         <v>88</v>
       </c>
-      <c r="M20" s="15" t="s">
+      <c r="M20" s="8" t="s">
         <v>86</v>
       </c>
-      <c r="N20" s="15" t="s">
+      <c r="N20" s="8" t="s">
         <v>87</v>
       </c>
-      <c r="O20" s="15"/>
-      <c r="P20" s="15"/>
-      <c r="Q20" s="15"/>
-      <c r="R20" s="3"/>
-      <c r="S20" s="6" t="s">
+      <c r="O20" s="8"/>
+      <c r="P20" s="8"/>
+      <c r="Q20" s="8"/>
+      <c r="R20" s="1"/>
+      <c r="S20" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T20" s="6" t="s">
+      <c r="T20" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U20" s="2"/>
-    </row>
-    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="14">
+      <c r="U20" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="21" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="7">
         <v>20</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="8" t="s">
         <v>53</v>
       </c>
-      <c r="C21" s="15" t="s">
+      <c r="C21" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="15" t="s">
+      <c r="D21" s="8" t="s">
         <v>54</v>
       </c>
-      <c r="E21" s="15" t="s">
+      <c r="E21" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F21" s="15" t="s">
+      <c r="F21" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G21" s="16"/>
-      <c r="H21" s="16"/>
-      <c r="I21" s="15"/>
-      <c r="J21" s="15"/>
-      <c r="K21" s="15"/>
-      <c r="L21" s="15" t="s">
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="8"/>
+      <c r="J21" s="8"/>
+      <c r="K21" s="8"/>
+      <c r="L21" s="8" t="s">
         <v>59</v>
       </c>
-      <c r="M21" s="15" t="s">
+      <c r="M21" s="8" t="s">
         <v>56</v>
       </c>
-      <c r="N21" s="15" t="s">
+      <c r="N21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="O21" s="15"/>
-      <c r="P21" s="15" t="s">
+      <c r="O21" s="8"/>
+      <c r="P21" s="8" t="s">
         <v>58</v>
       </c>
-      <c r="Q21" s="15"/>
-      <c r="R21" s="3"/>
-      <c r="S21" s="6" t="s">
+      <c r="Q21" s="8"/>
+      <c r="R21" s="1"/>
+      <c r="S21" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T21" s="6" t="s">
+      <c r="T21" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="14">
+      <c r="U21" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="22" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="7">
         <v>21</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="8" t="s">
         <v>60</v>
       </c>
-      <c r="C22" s="15" t="s">
+      <c r="C22" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D22" s="15" t="s">
+      <c r="D22" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G22" s="16"/>
-      <c r="H22" s="16"/>
-      <c r="I22" s="15"/>
-      <c r="J22" s="15"/>
-      <c r="K22" s="15"/>
-      <c r="L22" s="15" t="s">
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="8"/>
+      <c r="K22" s="8"/>
+      <c r="L22" s="8" t="s">
         <v>65</v>
       </c>
-      <c r="M22" s="15" t="s">
+      <c r="M22" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="N22" s="15" t="s">
+      <c r="N22" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="O22" s="15"/>
-      <c r="P22" s="15" t="s">
+      <c r="O22" s="8"/>
+      <c r="P22" s="8" t="s">
         <v>64</v>
       </c>
-      <c r="Q22" s="15"/>
-      <c r="R22" s="3"/>
-      <c r="S22" s="6" t="s">
+      <c r="Q22" s="8"/>
+      <c r="R22" s="1"/>
+      <c r="S22" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T22" s="6" t="s">
+      <c r="T22" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U22" s="2"/>
-    </row>
-    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="14">
+      <c r="U22" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="23" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="7">
         <v>22</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="C23" s="15" t="s">
+      <c r="C23" s="8" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="15" t="s">
+      <c r="D23" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="E23" s="15" t="s">
+      <c r="E23" s="8" t="s">
         <v>20</v>
       </c>
-      <c r="F23" s="15" t="s">
+      <c r="F23" s="8" t="s">
         <v>55</v>
       </c>
-      <c r="G23" s="16"/>
-      <c r="H23" s="16"/>
-      <c r="I23" s="15"/>
-      <c r="J23" s="15"/>
-      <c r="K23" s="15"/>
-      <c r="L23" s="15" t="s">
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="8"/>
+      <c r="J23" s="8"/>
+      <c r="K23" s="8"/>
+      <c r="L23" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="M23" s="15" t="s">
+      <c r="M23" s="8" t="s">
         <v>68</v>
       </c>
-      <c r="N23" s="15" t="s">
+      <c r="N23" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="O23" s="15"/>
-      <c r="P23" s="15" t="s">
+      <c r="O23" s="8"/>
+      <c r="P23" s="8" t="s">
         <v>70</v>
       </c>
-      <c r="Q23" s="15"/>
-      <c r="R23" s="3"/>
-      <c r="S23" s="6" t="s">
+      <c r="Q23" s="8"/>
+      <c r="R23" s="1"/>
+      <c r="S23" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T23" s="6" t="s">
+      <c r="T23" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="U23" s="2"/>
-    </row>
-    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="17">
+      <c r="U23" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="24" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="10">
         <v>23</v>
       </c>
-      <c r="B24" s="18" t="s">
+      <c r="B24" s="11" t="s">
         <v>117</v>
       </c>
-      <c r="C24" s="18" t="s">
+      <c r="C24" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D24" s="18" t="s">
+      <c r="D24" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="E24" s="18"/>
-      <c r="F24" s="18" t="s">
+      <c r="E24" s="11"/>
+      <c r="F24" s="11" t="s">
         <v>119</v>
       </c>
-      <c r="G24" s="18" t="s">
+      <c r="G24" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="H24" s="18" t="s">
+      <c r="H24" s="11" t="s">
         <v>121</v>
       </c>
-      <c r="I24" s="18"/>
-      <c r="J24" s="18"/>
-      <c r="K24" s="18"/>
-      <c r="L24" s="18" t="s">
+      <c r="I24" s="11"/>
+      <c r="J24" s="11"/>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11" t="s">
         <v>122</v>
       </c>
-      <c r="M24" s="18"/>
-      <c r="N24" s="18" t="s">
+      <c r="M24" s="11"/>
+      <c r="N24" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="O24" s="18" t="s">
+      <c r="O24" s="11" t="s">
         <v>124</v>
       </c>
-      <c r="P24" s="18"/>
-      <c r="Q24" s="18" t="s">
+      <c r="P24" s="11"/>
+      <c r="Q24" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="R24" s="20" t="s">
+      <c r="R24" s="13" t="s">
         <v>126</v>
       </c>
-      <c r="S24" s="26" t="s">
+      <c r="S24" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="T24" s="26" t="s">
+      <c r="T24" s="15" t="s">
         <v>236</v>
       </c>
-      <c r="U24" s="2"/>
-    </row>
-    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="23">
+      <c r="U24" s="1" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="25" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="16">
         <v>24</v>
       </c>
-      <c r="B25" s="24" t="s">
+      <c r="B25" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="24" t="s">
+      <c r="C25" s="17" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="24" t="s">
+      <c r="D25" s="17" t="s">
         <v>30</v>
       </c>
-      <c r="E25" s="24" t="s">
+      <c r="E25" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="F25" s="24" t="s">
+      <c r="F25" s="17" t="s">
         <v>31</v>
       </c>
-      <c r="G25" s="24" t="s">
+      <c r="G25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="H25" s="24" t="s">
+      <c r="H25" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24" t="s">
+      <c r="I25" s="17"/>
+      <c r="J25" s="17"/>
+      <c r="K25" s="17"/>
+      <c r="L25" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24" t="s">
+      <c r="M25" s="17"/>
+      <c r="N25" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="25" t="s">
+      <c r="O25" s="17"/>
+      <c r="P25" s="17"/>
+      <c r="Q25" s="17"/>
+      <c r="R25" s="18" t="s">
         <v>221</v>
       </c>
-      <c r="S25" s="27" t="s">
+      <c r="S25" s="19" t="s">
         <v>236</v>
       </c>
-      <c r="T25" s="27" t="s">
+      <c r="T25" s="19" t="s">
         <v>264</v>
       </c>
-      <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="17">
+      <c r="U25" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="26" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="10">
         <v>25</v>
       </c>
-      <c r="B26" s="18" t="s">
+      <c r="B26" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="18" t="s">
+      <c r="C26" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D26" s="18" t="s">
+      <c r="D26" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F26" s="18" t="s">
+      <c r="F26" s="11" t="s">
         <v>21</v>
       </c>
-      <c r="G26" s="18" t="s">
+      <c r="G26" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="H26" s="18" t="s">
+      <c r="H26" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="I26" s="18"/>
-      <c r="J26" s="18"/>
-      <c r="K26" s="18"/>
-      <c r="L26" s="18"/>
-      <c r="M26" s="18"/>
-      <c r="N26" s="18"/>
-      <c r="O26" s="18"/>
-      <c r="P26" s="18"/>
-      <c r="Q26" s="18" t="s">
+      <c r="I26" s="11"/>
+      <c r="J26" s="11"/>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11"/>
+      <c r="M26" s="11"/>
+      <c r="N26" s="11"/>
+      <c r="O26" s="11"/>
+      <c r="P26" s="11"/>
+      <c r="Q26" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="R26" s="21" t="s">
+      <c r="R26" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="S26" s="22" t="s">
+      <c r="S26" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="T26" s="22" t="s">
+      <c r="T26" s="15" t="s">
         <v>233</v>
       </c>
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="4">
+      <c r="U26" s="15" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="27" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="2">
         <v>26</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="C27" s="3" t="s">
+      <c r="C27" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D27" s="3" t="s">
+      <c r="D27" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="E27" s="3"/>
-      <c r="F27" s="3" t="s">
+      <c r="E27" s="1"/>
+      <c r="F27" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="G27" s="9" t="s">
+      <c r="G27" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="H27" s="3" t="s">
+      <c r="H27" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="I27" s="3"/>
-      <c r="J27" s="3"/>
-      <c r="K27" s="3"/>
-      <c r="L27" s="3" t="s">
+      <c r="I27" s="1"/>
+      <c r="J27" s="1"/>
+      <c r="K27" s="1"/>
+      <c r="L27" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="M27" s="3"/>
-      <c r="N27" s="3" t="s">
+      <c r="M27" s="1"/>
+      <c r="N27" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="O27" s="3"/>
-      <c r="P27" s="3"/>
-      <c r="Q27" s="3" t="s">
+      <c r="O27" s="1"/>
+      <c r="P27" s="1"/>
+      <c r="Q27" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="R27" s="3"/>
-      <c r="S27" s="6" t="s">
+      <c r="R27" s="1"/>
+      <c r="S27" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T27" s="3" t="s">
+      <c r="T27" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="4">
+      <c r="U27" s="4" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="28" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="2">
         <v>27</v>
       </c>
-      <c r="B28" s="3" t="s">
+      <c r="B28" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="C28" s="3" t="s">
+      <c r="C28" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D28" s="3" t="s">
+      <c r="D28" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="E28" s="3"/>
-      <c r="F28" s="3"/>
-      <c r="G28" s="9"/>
-      <c r="H28" s="3"/>
-      <c r="I28" s="3"/>
-      <c r="J28" s="3"/>
-      <c r="K28" s="3"/>
-      <c r="L28" s="3" t="s">
+      <c r="E28" s="1"/>
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+      <c r="I28" s="1"/>
+      <c r="J28" s="1"/>
+      <c r="K28" s="1"/>
+      <c r="L28" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="M28" s="3" t="s">
+      <c r="M28" s="1" t="s">
         <v>129</v>
       </c>
-      <c r="N28" s="3"/>
-      <c r="O28" s="3"/>
-      <c r="P28" s="3"/>
-      <c r="Q28" s="3" t="s">
+      <c r="N28" s="1"/>
+      <c r="O28" s="1"/>
+      <c r="P28" s="1"/>
+      <c r="Q28" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="R28" s="3"/>
-      <c r="S28" s="3" t="s">
+      <c r="R28" s="1"/>
+      <c r="S28" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="T28" s="42" t="s">
+      <c r="T28" s="27" t="s">
         <v>270</v>
       </c>
-      <c r="U28" s="2"/>
-    </row>
-    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="4">
+      <c r="U28" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="29" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="2">
         <v>28</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C29" s="3" t="s">
+      <c r="C29" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D29" s="3" t="s">
+      <c r="D29" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="E29" s="3"/>
-      <c r="F29" s="3"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="3"/>
-      <c r="I29" s="3"/>
-      <c r="J29" s="3"/>
-      <c r="K29" s="3"/>
-      <c r="L29" s="3" t="s">
+      <c r="E29" s="1"/>
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+      <c r="I29" s="1"/>
+      <c r="J29" s="1"/>
+      <c r="K29" s="1"/>
+      <c r="L29" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="M29" s="3" t="s">
+      <c r="M29" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="N29" s="3"/>
-      <c r="O29" s="3"/>
-      <c r="P29" s="3"/>
-      <c r="Q29" s="3" t="s">
+      <c r="N29" s="1"/>
+      <c r="O29" s="1"/>
+      <c r="P29" s="1"/>
+      <c r="Q29" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="R29" s="3"/>
-      <c r="S29" s="3" t="s">
+      <c r="R29" s="1"/>
+      <c r="S29" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="T29" s="42" t="s">
+      <c r="T29" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="U29" s="2"/>
-    </row>
-    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="4">
+      <c r="U29" s="1" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="30" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="2">
         <v>29</v>
       </c>
-      <c r="B30" s="3" t="s">
+      <c r="B30" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C30" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="3" t="s">
+      <c r="D30" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="E30" s="3"/>
-      <c r="F30" s="3"/>
-      <c r="G30" s="9"/>
-      <c r="H30" s="3"/>
-      <c r="I30" s="3"/>
-      <c r="J30" s="3"/>
-      <c r="K30" s="3" t="s">
+      <c r="E30" s="1"/>
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+      <c r="I30" s="1"/>
+      <c r="J30" s="1"/>
+      <c r="K30" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L30" s="3" t="s">
+      <c r="L30" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="M30" s="3"/>
-      <c r="N30" s="3" t="s">
+      <c r="M30" s="1"/>
+      <c r="N30" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="O30" s="3"/>
-      <c r="P30" s="3"/>
-      <c r="Q30" s="3" t="s">
+      <c r="O30" s="1"/>
+      <c r="P30" s="1"/>
+      <c r="Q30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="R30" s="3"/>
-      <c r="S30" s="6" t="s">
+      <c r="R30" s="1"/>
+      <c r="S30" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T30" s="42" t="s">
+      <c r="T30" s="27" t="s">
         <v>263</v>
       </c>
-      <c r="U30" s="2"/>
-    </row>
-    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="4">
+      <c r="U30" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="31" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="2">
         <v>30</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C31" s="3" t="s">
+      <c r="C31" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="D31" s="1" t="s">
         <v>140</v>
       </c>
-      <c r="E31" s="3"/>
-      <c r="F31" s="3"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="3"/>
-      <c r="I31" s="3"/>
-      <c r="J31" s="3"/>
-      <c r="K31" s="3" t="s">
+      <c r="E31" s="1"/>
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+      <c r="I31" s="1"/>
+      <c r="J31" s="1"/>
+      <c r="K31" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="L31" s="3" t="s">
+      <c r="L31" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="M31" s="3"/>
-      <c r="N31" s="3" t="s">
+      <c r="M31" s="1"/>
+      <c r="N31" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="O31" s="3"/>
-      <c r="P31" s="3"/>
-      <c r="Q31" s="3"/>
-      <c r="R31" s="3"/>
-      <c r="S31" s="6" t="s">
+      <c r="O31" s="1"/>
+      <c r="P31" s="1"/>
+      <c r="Q31" s="1"/>
+      <c r="R31" s="1"/>
+      <c r="S31" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="T31" s="42" t="s">
+      <c r="T31" s="27" t="s">
         <v>272</v>
       </c>
-      <c r="U31" s="2"/>
-    </row>
-    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="4">
+      <c r="U31" s="4" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="32" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="2">
         <v>31</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="C32" s="3" t="s">
+      <c r="C32" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="D32" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="E32" s="3"/>
-      <c r="F32" s="3"/>
-      <c r="G32" s="9"/>
-      <c r="H32" s="3"/>
-      <c r="I32" s="3"/>
-      <c r="J32" s="3"/>
-      <c r="K32" s="3" t="s">
+      <c r="E32" s="1"/>
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="L32" s="3"/>
-      <c r="M32" s="3" t="s">
+      <c r="L32" s="1"/>
+      <c r="M32" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="N32" s="3" t="s">
+      <c r="N32" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="O32" s="3"/>
-      <c r="P32" s="3"/>
-      <c r="Q32" s="3" t="s">
+      <c r="O32" s="1"/>
+      <c r="P32" s="1"/>
+      <c r="Q32" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="R32" s="3"/>
-      <c r="S32" s="6" t="s">
+      <c r="R32" s="1"/>
+      <c r="S32" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T32" s="42" t="s">
+      <c r="T32" s="27" t="s">
         <v>271</v>
       </c>
-      <c r="U32" s="2"/>
-    </row>
-    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="4">
+      <c r="U32" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="33" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="2">
         <v>32</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="4" t="s">
         <v>217</v>
       </c>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="3"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
-      <c r="M33" s="3"/>
-      <c r="N33" s="3"/>
-      <c r="O33" s="3"/>
-      <c r="P33" s="3"/>
-      <c r="Q33" s="3"/>
-      <c r="R33" s="3"/>
-      <c r="S33" s="6" t="s">
+      <c r="C33" s="1"/>
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+      <c r="K33" s="1"/>
+      <c r="L33" s="1"/>
+      <c r="M33" s="1"/>
+      <c r="N33" s="1"/>
+      <c r="O33" s="1"/>
+      <c r="P33" s="1"/>
+      <c r="Q33" s="1"/>
+      <c r="R33" s="1"/>
+      <c r="S33" s="4" t="s">
         <v>236</v>
       </c>
-      <c r="T33" s="6" t="s">
+      <c r="T33" s="4" t="s">
         <v>263</v>
       </c>
-      <c r="U33" s="3"/>
-    </row>
-    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="4">
+      <c r="U33" s="4" t="s">
+        <v>263</v>
+      </c>
+    </row>
+    <row r="34" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="2">
         <v>33</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="1" t="s">
         <v>150</v>
       </c>
-      <c r="C34" s="3" t="s">
+      <c r="C34" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D34" s="3" t="s">
+      <c r="D34" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="3"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3" t="s">
+      <c r="E34" s="1"/>
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
-      <c r="M34" s="3"/>
-      <c r="N34" s="3" t="s">
+      <c r="K34" s="1"/>
+      <c r="L34" s="1"/>
+      <c r="M34" s="1"/>
+      <c r="N34" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="O34" s="3"/>
-      <c r="P34" s="3"/>
-      <c r="Q34" s="3" t="s">
+      <c r="O34" s="1"/>
+      <c r="P34" s="1"/>
+      <c r="Q34" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="R34" s="3"/>
-      <c r="S34" s="6" t="s">
+      <c r="R34" s="1"/>
+      <c r="S34" s="4" t="s">
         <v>230</v>
       </c>
-      <c r="T34" s="3" t="s">
+      <c r="T34" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="U34" s="2"/>
-    </row>
-    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="17">
+      <c r="U34" s="4" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="35" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="10">
         <v>34</v>
       </c>
-      <c r="B35" s="18" t="s">
+      <c r="B35" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C35" s="18" t="s">
+      <c r="C35" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D35" s="18" t="s">
+      <c r="D35" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="18" t="s">
+      <c r="E35" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F35" s="18"/>
-      <c r="G35" s="18"/>
-      <c r="H35" s="18"/>
-      <c r="I35" s="18"/>
-      <c r="J35" s="18"/>
-      <c r="K35" s="18"/>
-      <c r="L35" s="18"/>
-      <c r="M35" s="18" t="s">
+      <c r="F35" s="11"/>
+      <c r="G35" s="11"/>
+      <c r="H35" s="11"/>
+      <c r="I35" s="11"/>
+      <c r="J35" s="11"/>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11"/>
+      <c r="M35" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="N35" s="18"/>
-      <c r="O35" s="18"/>
-      <c r="P35" s="18"/>
-      <c r="Q35" s="18"/>
-      <c r="R35" s="22" t="s">
+      <c r="N35" s="11"/>
+      <c r="O35" s="11"/>
+      <c r="P35" s="11"/>
+      <c r="Q35" s="11"/>
+      <c r="R35" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="S35" s="22" t="s">
+      <c r="S35" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="T35" s="22"/>
-      <c r="U35" s="2"/>
-    </row>
-    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="17">
+      <c r="T35" s="15"/>
+      <c r="U35" s="15" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="36" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="10">
         <v>35</v>
       </c>
-      <c r="B36" s="18" t="s">
+      <c r="B36" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="C36" s="18" t="s">
+      <c r="C36" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="D36" s="18" t="s">
+      <c r="D36" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E36" s="18" t="s">
+      <c r="E36" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="F36" s="18"/>
-      <c r="G36" s="18"/>
-      <c r="H36" s="18"/>
-      <c r="I36" s="18"/>
-      <c r="J36" s="18"/>
-      <c r="K36" s="18"/>
-      <c r="L36" s="18"/>
-      <c r="M36" s="18" t="s">
+      <c r="F36" s="11"/>
+      <c r="G36" s="11"/>
+      <c r="H36" s="11"/>
+      <c r="I36" s="11"/>
+      <c r="J36" s="11"/>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11"/>
+      <c r="M36" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="N36" s="18"/>
-      <c r="O36" s="18"/>
-      <c r="P36" s="18"/>
-      <c r="Q36" s="18" t="s">
+      <c r="N36" s="11"/>
+      <c r="O36" s="11"/>
+      <c r="P36" s="11"/>
+      <c r="Q36" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="R36" s="22" t="s">
+      <c r="R36" s="15" t="s">
         <v>223</v>
       </c>
-      <c r="S36" s="22" t="s">
+      <c r="S36" s="15" t="s">
         <v>231</v>
       </c>
-      <c r="T36" s="22"/>
-      <c r="U36" s="2"/>
-    </row>
-    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="4">
+      <c r="T36" s="15"/>
+      <c r="U36" s="15" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="37" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="2">
         <v>36</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="C37" s="3" t="s">
+      <c r="C37" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D37" s="3" t="s">
+      <c r="D37" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="E37" s="3"/>
-      <c r="F37" s="3"/>
-      <c r="G37" s="9"/>
-      <c r="H37" s="3"/>
-      <c r="I37" s="3"/>
-      <c r="J37" s="3" t="s">
+      <c r="E37" s="1"/>
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="K37" s="3"/>
-      <c r="L37" s="3"/>
-      <c r="M37" s="3" t="s">
+      <c r="K37" s="1"/>
+      <c r="L37" s="1"/>
+      <c r="M37" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N37" s="3" t="s">
+      <c r="N37" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="O37" s="3"/>
-      <c r="P37" s="3"/>
-      <c r="Q37" s="3" t="s">
+      <c r="O37" s="1"/>
+      <c r="P37" s="1"/>
+      <c r="Q37" s="1" t="s">
         <v>160</v>
       </c>
-      <c r="R37" s="3"/>
-      <c r="S37" s="6" t="s">
+      <c r="R37" s="1"/>
+      <c r="S37" s="4" t="s">
         <v>229</v>
       </c>
-      <c r="T37" s="3" t="s">
+      <c r="T37" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="U37" s="2"/>
-    </row>
-    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="4">
+      <c r="U37" s="4" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="38" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="2">
         <v>37</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C38" s="3" t="s">
+      <c r="C38" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="D38" s="3" t="s">
+      <c r="D38" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="E38" s="3"/>
-      <c r="F38" s="3"/>
-      <c r="G38" s="9"/>
-      <c r="H38" s="3"/>
-      <c r="I38" s="3"/>
-      <c r="J38" s="3"/>
-      <c r="K38" s="3" t="s">
+      <c r="E38" s="1"/>
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+      <c r="K38" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="L38" s="3" t="s">
+      <c r="L38" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="M38" s="3"/>
-      <c r="N38" s="3" t="s">
+      <c r="M38" s="1"/>
+      <c r="N38" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="O38" s="3"/>
-      <c r="P38" s="3"/>
-      <c r="Q38" s="3"/>
-      <c r="R38" s="3"/>
-      <c r="S38" s="6" t="s">
+      <c r="O38" s="1"/>
+      <c r="P38" s="1"/>
+      <c r="Q38" s="1"/>
+      <c r="R38" s="1"/>
+      <c r="S38" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="T38" s="42" t="s">
+      <c r="T38" s="27" t="s">
         <v>266</v>
       </c>
-      <c r="U38" s="2"/>
-    </row>
-    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="30">
+      <c r="U38" s="4" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="39" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="22">
         <v>38</v>
       </c>
-      <c r="B39" s="28" t="s">
+      <c r="B39" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="C39" s="29" t="s">
+      <c r="C39" s="21" t="s">
         <v>218</v>
       </c>
-      <c r="D39" s="30"/>
-      <c r="E39" s="30"/>
-      <c r="F39" s="30"/>
-      <c r="G39" s="31"/>
-      <c r="H39" s="30"/>
-      <c r="I39" s="30"/>
-      <c r="J39" s="30"/>
-      <c r="K39" s="30"/>
-      <c r="L39" s="30"/>
-      <c r="M39" s="30"/>
-      <c r="N39" s="30"/>
-      <c r="O39" s="30"/>
-      <c r="P39" s="30"/>
-      <c r="Q39" s="30"/>
-      <c r="R39" s="30"/>
-      <c r="S39" s="28" t="s">
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="22"/>
+      <c r="G39" s="22"/>
+      <c r="H39" s="22"/>
+      <c r="I39" s="22"/>
+      <c r="J39" s="22"/>
+      <c r="K39" s="22"/>
+      <c r="L39" s="22"/>
+      <c r="M39" s="22"/>
+      <c r="N39" s="22"/>
+      <c r="O39" s="22"/>
+      <c r="P39" s="22"/>
+      <c r="Q39" s="22"/>
+      <c r="R39" s="22"/>
+      <c r="S39" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="T39" s="28" t="s">
+      <c r="T39" s="20" t="s">
         <v>215</v>
       </c>
-      <c r="U39" s="2"/>
-    </row>
-    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="2"/>
-      <c r="B40" s="2"/>
-      <c r="C40" s="2"/>
-      <c r="D40" s="2"/>
-      <c r="E40" s="2"/>
-      <c r="F40" s="2"/>
-      <c r="G40" s="9"/>
-      <c r="H40" s="2"/>
-      <c r="I40" s="2"/>
-      <c r="J40" s="2"/>
-      <c r="K40" s="2"/>
-      <c r="L40" s="2"/>
-      <c r="M40" s="2"/>
-      <c r="N40" s="2"/>
-      <c r="O40" s="2"/>
-      <c r="P40" s="2"/>
-      <c r="Q40" s="2"/>
-      <c r="R40" s="2"/>
-      <c r="S40" s="3"/>
-      <c r="T40" s="3"/>
-      <c r="U40" s="2"/>
-    </row>
-    <row r="41" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A41" s="2"/>
-      <c r="B41" s="2"/>
-      <c r="C41" s="2"/>
-      <c r="D41" s="2"/>
-      <c r="E41" s="2"/>
-      <c r="F41" s="2"/>
-      <c r="G41" s="11"/>
-      <c r="H41" s="2"/>
-      <c r="I41" s="2"/>
-      <c r="J41" s="2"/>
-      <c r="K41" s="2"/>
-      <c r="L41" s="2"/>
-      <c r="M41" s="2"/>
-      <c r="N41" s="2"/>
-      <c r="O41" s="2"/>
-      <c r="P41" s="2"/>
-      <c r="Q41" s="2"/>
-      <c r="R41" s="43" t="s">
+      <c r="U39" s="20" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="40" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A40" s="1"/>
+      <c r="B40" s="1"/>
+      <c r="C40" s="1"/>
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+      <c r="K40" s="1"/>
+      <c r="L40" s="1"/>
+      <c r="M40" s="1"/>
+      <c r="N40" s="1"/>
+      <c r="O40" s="1"/>
+      <c r="P40" s="1"/>
+      <c r="Q40" s="1"/>
+      <c r="R40" s="1"/>
+      <c r="S40" s="1"/>
+      <c r="T40" s="1"/>
+      <c r="U40" s="1"/>
+    </row>
+    <row r="41" spans="1:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A41" s="1"/>
+      <c r="B41" s="1"/>
+      <c r="C41" s="1"/>
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="F41" s="1"/>
+      <c r="G41" s="2"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+      <c r="K41" s="1"/>
+      <c r="L41" s="1"/>
+      <c r="M41" s="1"/>
+      <c r="N41" s="1"/>
+      <c r="O41" s="1"/>
+      <c r="P41" s="1"/>
+      <c r="Q41" s="1"/>
+      <c r="R41" s="28" t="s">
         <v>253</v>
       </c>
-      <c r="S41" s="37" t="s">
+      <c r="S41" s="23" t="s">
         <v>237</v>
       </c>
-      <c r="T41" s="37" t="s">
+      <c r="T41" s="23" t="s">
         <v>238</v>
       </c>
-      <c r="U41" s="2"/>
-    </row>
-    <row r="42" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A42" s="2"/>
-      <c r="B42" s="2"/>
-      <c r="C42" s="2"/>
-      <c r="D42" s="2"/>
-      <c r="E42" s="2"/>
-      <c r="F42" s="2"/>
-      <c r="G42" s="11"/>
-      <c r="H42" s="2"/>
-      <c r="I42" s="2"/>
-      <c r="J42" s="2"/>
-      <c r="K42" s="2"/>
-      <c r="L42" s="2"/>
-      <c r="M42" s="2"/>
-      <c r="N42" s="2"/>
-      <c r="O42" s="2"/>
-      <c r="P42" s="2"/>
-      <c r="Q42" s="2"/>
-      <c r="R42" s="40">
+      <c r="U41" s="1"/>
+    </row>
+    <row r="42" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A42" s="1"/>
+      <c r="B42" s="1"/>
+      <c r="C42" s="1"/>
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="F42" s="1"/>
+      <c r="G42" s="2"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+      <c r="K42" s="1"/>
+      <c r="L42" s="1"/>
+      <c r="M42" s="1"/>
+      <c r="N42" s="1"/>
+      <c r="O42" s="1"/>
+      <c r="P42" s="1"/>
+      <c r="Q42" s="1"/>
+      <c r="R42" s="25">
         <v>1</v>
       </c>
-      <c r="S42" s="6" t="s">
+      <c r="S42" s="4" t="s">
         <v>242</v>
       </c>
-      <c r="T42" s="6" t="s">
+      <c r="T42" s="4" t="s">
         <v>257</v>
       </c>
-      <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A43" s="2"/>
-      <c r="B43" s="2"/>
-      <c r="C43" s="2"/>
-      <c r="D43" s="2"/>
-      <c r="E43" s="2"/>
-      <c r="F43" s="2"/>
-      <c r="G43" s="11"/>
-      <c r="H43" s="2"/>
-      <c r="I43" s="2"/>
-      <c r="J43" s="2"/>
-      <c r="K43" s="2"/>
-      <c r="L43" s="2"/>
-      <c r="M43" s="2"/>
-      <c r="N43" s="2"/>
-      <c r="O43" s="2"/>
-      <c r="P43" s="2"/>
-      <c r="Q43" s="2"/>
-      <c r="R43" s="40">
+      <c r="U42" s="1"/>
+    </row>
+    <row r="43" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A43" s="1"/>
+      <c r="B43" s="1"/>
+      <c r="C43" s="1"/>
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="F43" s="1"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+      <c r="K43" s="1"/>
+      <c r="L43" s="1"/>
+      <c r="M43" s="1"/>
+      <c r="N43" s="1"/>
+      <c r="O43" s="1"/>
+      <c r="P43" s="1"/>
+      <c r="Q43" s="1"/>
+      <c r="R43" s="25">
         <v>2</v>
       </c>
-      <c r="S43" s="6" t="s">
+      <c r="S43" s="4" t="s">
         <v>243</v>
       </c>
-      <c r="T43" s="6" t="s">
+      <c r="T43" s="4" t="s">
         <v>215</v>
       </c>
-      <c r="U43" s="2"/>
-    </row>
-    <row r="44" spans="1:21" ht="15" x14ac:dyDescent="0.25">
-      <c r="A44" s="2"/>
-      <c r="B44" s="2"/>
-      <c r="C44" s="2"/>
-      <c r="D44" s="2"/>
-      <c r="E44" s="2"/>
-      <c r="F44" s="2"/>
-      <c r="G44" s="11"/>
-      <c r="H44" s="2"/>
-      <c r="I44" s="2"/>
-      <c r="J44" s="2"/>
-      <c r="K44" s="2"/>
-      <c r="L44" s="2"/>
-      <c r="M44" s="2"/>
-      <c r="N44" s="2"/>
-      <c r="O44" s="2"/>
-      <c r="P44" s="2"/>
-      <c r="Q44" s="2"/>
-      <c r="R44" s="40">
+      <c r="U43" s="1"/>
+    </row>
+    <row r="44" spans="1:21" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A44" s="1"/>
+      <c r="B44" s="1"/>
+      <c r="C44" s="1"/>
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+      <c r="F44" s="1"/>
+      <c r="G44" s="2"/>
+      <c r="H44" s="1"/>
+      <c r="I44" s="1"/>
+      <c r="J44" s="1"/>
+      <c r="K44" s="1"/>
+      <c r="L44" s="1"/>
+      <c r="M44" s="1"/>
+      <c r="N44" s="1"/>
+      <c r="O44" s="1"/>
+      <c r="P44" s="1"/>
+      <c r="Q44" s="1"/>
+      <c r="R44" s="25">
         <v>3</v>
       </c>
-      <c r="S44" s="6" t="s">
+      <c r="S44" s="4" t="s">
         <v>244</v>
       </c>
-      <c r="T44" s="42" t="s">
+      <c r="T44" s="27" t="s">
         <v>265</v>
       </c>
-      <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R45" s="40">
+      <c r="U44" s="1"/>
+    </row>
+    <row r="45" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R45" s="25">
         <v>4</v>
       </c>
-      <c r="S45" s="6" t="s">
+      <c r="S45" s="4" t="s">
         <v>245</v>
       </c>
-      <c r="T45" s="6" t="s">
+      <c r="T45" s="4" t="s">
         <v>259</v>
       </c>
     </row>
-    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R46" s="40">
+    <row r="46" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R46" s="25">
         <v>5</v>
       </c>
-      <c r="S46" s="6" t="s">
+      <c r="S46" s="4" t="s">
         <v>246</v>
       </c>
-      <c r="T46" s="6" t="s">
+      <c r="T46" s="4" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R47" s="40">
+    <row r="47" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R47" s="25">
         <v>6</v>
       </c>
-      <c r="S47" s="6" t="s">
+      <c r="S47" s="4" t="s">
         <v>247</v>
       </c>
-      <c r="T47" s="6" t="s">
+      <c r="T47" s="4" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R48" s="40">
+    <row r="48" spans="1:21" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R48" s="25">
         <v>7</v>
       </c>
-      <c r="S48" s="6" t="s">
+      <c r="S48" s="4" t="s">
         <v>262</v>
       </c>
-      <c r="T48" s="42" t="s">
+      <c r="T48" s="27" t="s">
         <v>269</v>
       </c>
     </row>
-    <row r="49" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R49" s="40">
+    <row r="49" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R49" s="25">
         <v>8</v>
       </c>
-      <c r="S49" s="41" t="s">
+      <c r="S49" s="26" t="s">
         <v>248</v>
       </c>
-      <c r="T49" s="42" t="s">
+      <c r="T49" s="27" t="s">
         <v>261</v>
       </c>
     </row>
-    <row r="50" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R50" s="40">
+    <row r="50" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R50" s="25">
         <v>9</v>
       </c>
-      <c r="S50" s="42" t="s">
+      <c r="S50" s="27" t="s">
         <v>255</v>
       </c>
-      <c r="T50" s="42" t="s">
+      <c r="T50" s="27" t="s">
         <v>268</v>
       </c>
     </row>
-    <row r="51" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R51" s="40">
+    <row r="51" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R51" s="25">
         <v>10</v>
       </c>
-      <c r="S51" s="42" t="s">
+      <c r="S51" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="T51" s="42" t="s">
+      <c r="T51" s="27" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="52" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R52" s="40">
+    <row r="52" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R52" s="25">
         <v>11</v>
       </c>
-      <c r="S52" s="42" t="s">
+      <c r="S52" s="27" t="s">
         <v>252</v>
       </c>
-      <c r="T52" s="42" t="s">
+      <c r="T52" s="27" t="s">
         <v>267</v>
       </c>
     </row>
-    <row r="53" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R53" s="40">
+    <row r="53" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R53" s="25">
         <v>12</v>
       </c>
-      <c r="S53" s="42" t="s">
+      <c r="S53" s="27" t="s">
         <v>251</v>
       </c>
-      <c r="T53" s="42" t="s">
+      <c r="T53" s="27" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="54" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="R54" s="40">
+    <row r="54" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R54" s="25">
         <v>13</v>
       </c>
-      <c r="S54" s="41" t="s">
+      <c r="S54" s="26" t="s">
         <v>249</v>
       </c>
-      <c r="T54" s="6" t="s">
+      <c r="T54" s="4" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="55" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S55" s="6"/>
-      <c r="T55" s="6"/>
-    </row>
-    <row r="56" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="S56" s="6"/>
+    <row r="55" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S55" s="4"/>
+      <c r="T55" s="4"/>
+    </row>
+    <row r="56" spans="18:20" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="S56" s="4"/>
     </row>
   </sheetData>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:S38">
     <sortCondition ref="A6:A38"/>
   </sortState>
+  <mergeCells count="1">
+    <mergeCell ref="U5:U8"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>

</xml_diff>